<commit_message>
add col SoQtin and SoQPsu for THOI SU report
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateTS.xlsx
+++ b/ATV_Allowance/Templates/TemplateTS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Đài Phát thanh - Truyền hình An Giang</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>(PV)</t>
+  </si>
+  <si>
+    <t>Q.Tin</t>
+  </si>
+  <si>
+    <t>Q.P/sự</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,6 +228,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -236,12 +251,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,10 +535,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,93 +548,99 @@
     <col min="3" max="3" width="6.28515625" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" customWidth="1"/>
+    <col min="8" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
     <col min="11" max="11" width="7.140625" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-    </row>
-    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+    </row>
+    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="10" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="L3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="M3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="N3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="O3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="P3" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
+    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
@@ -638,20 +653,26 @@
       <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="18"/>
-    </row>
-    <row r="5" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="21"/>
+    </row>
+    <row r="5" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
       <c r="C5" s="11"/>
@@ -664,40 +685,44 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="12"/>
+      <c r="M5" s="11"/>
       <c r="N5" s="11"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="O5" s="12"/>
+      <c r="P5" s="11"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7"/>
-      <c r="N7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8"/>
-      <c r="N8" s="5" t="s">
+      <c r="P8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9" s="6" t="s">
         <v>17</v>
@@ -705,27 +730,27 @@
       <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>19</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:P1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="C3:J3"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="N3:N4"/>
-    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add KHK to report TS PV
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateTS.xlsx
+++ b/ATV_Allowance/Templates/TemplateTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="PV" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>Đài Phát thanh - Truyền hình An Giang</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>KHỐI HẬU KỲ</t>
+  </si>
+  <si>
+    <t>Bộ phận</t>
+  </si>
+  <si>
+    <t>Tỉ lệ % trên mức thù lao</t>
+  </si>
+  <si>
+    <t>TỔNG CỘNG</t>
   </si>
 </sst>
 </file>
@@ -148,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -180,11 +192,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,20 +294,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,10 +659,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,89 +679,89 @@
     <col min="12" max="12" width="5.7109375" customWidth="1"/>
     <col min="13" max="13" width="7.140625" customWidth="1"/>
     <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="6" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="6" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
     </row>
     <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
@@ -689,12 +786,12 @@
       <c r="J4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="21"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
@@ -715,10 +812,10 @@
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="19"/>
+      <c r="A6" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="31"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -734,36 +831,261 @@
       <c r="O6" s="14"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O7" s="16"/>
-      <c r="P7" s="17" t="s">
+    <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="22"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="22"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="22"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="22"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="22"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="22"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="22"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="36"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="21"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="23"/>
+    </row>
+    <row r="18" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O18" s="16"/>
+      <c r="P18" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="P8" s="4" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="P19" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9" s="5" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E20" t="s">
         <v>17</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L20" t="s">
         <v>18</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P20" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="23">
+    <mergeCell ref="A17:N17"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="C14:N14"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="C12:N12"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
@@ -788,8 +1110,8 @@
   </sheetPr>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,89 +1128,89 @@
     <col min="12" max="12" width="5.7109375" customWidth="1"/>
     <col min="13" max="13" width="7.140625" customWidth="1"/>
     <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="6" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="6" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
     </row>
     <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="18" t="s">
         <v>13</v>
       </c>
@@ -913,12 +1235,12 @@
       <c r="J4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="21"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
@@ -939,10 +1261,10 @@
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>

</xml_diff>

<commit_message>
add KTD to report TS
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateTS.xlsx
+++ b/ATV_Allowance/Templates/TemplateTS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\job\ATV-Allowance\ATV-Allowance\ATV_Allowance\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\ATV-Allowance\ATV-Allowance\ATV_Allowance\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PV" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>Đài Phát thanh - Truyền hình An Giang</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>TỔNG CỘNG</t>
-  </si>
-  <si>
-    <t>12/2018</t>
   </si>
   <si>
     <t>Ban biên tập                                                                    Kế toán</t>
@@ -130,13 +127,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -144,7 +141,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -152,7 +149,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -160,7 +157,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -187,12 +184,6 @@
     <font>
       <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -266,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -281,11 +272,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -303,13 +294,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -337,7 +328,6 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -348,7 +338,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -366,7 +355,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -375,13 +364,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -701,103 +690,103 @@
       <selection activeCell="O5" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="7" width="5.5703125" customWidth="1"/>
-    <col min="8" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="5.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" customWidth="1"/>
+    <col min="3" max="3" width="6.25" customWidth="1"/>
+    <col min="4" max="4" width="5.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="7" width="5.625" customWidth="1"/>
+    <col min="8" max="9" width="8.75" customWidth="1"/>
+    <col min="10" max="10" width="7.875" customWidth="1"/>
+    <col min="11" max="11" width="7.125" customWidth="1"/>
+    <col min="12" max="12" width="5.75" customWidth="1"/>
+    <col min="13" max="13" width="7.125" customWidth="1"/>
+    <col min="14" max="14" width="6.75" customWidth="1"/>
+    <col min="15" max="15" width="13.125" style="6" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-    </row>
-    <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+    </row>
+    <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="M3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="39" t="s">
+      <c r="O3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
@@ -822,14 +811,14 @@
       <c r="J4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="38"/>
-    </row>
-    <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="36"/>
+    </row>
+    <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="7"/>
@@ -847,11 +836,11 @@
       <c r="O5" s="8"/>
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -867,19 +856,19 @@
       <c r="O6" s="14"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O7" s="16"/>
       <c r="P7" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="P8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" s="5" t="s">
         <v>16</v>
@@ -921,107 +910,107 @@
   </sheetPr>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="O5" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="7" width="5.5703125" customWidth="1"/>
-    <col min="8" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="5.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" customWidth="1"/>
+    <col min="3" max="3" width="6.25" customWidth="1"/>
+    <col min="4" max="4" width="5.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="7" width="5.625" customWidth="1"/>
+    <col min="8" max="9" width="8.75" customWidth="1"/>
+    <col min="10" max="10" width="7.875" customWidth="1"/>
+    <col min="11" max="11" width="7.125" customWidth="1"/>
+    <col min="12" max="12" width="5.75" customWidth="1"/>
+    <col min="13" max="13" width="7.125" customWidth="1"/>
+    <col min="14" max="14" width="6.75" customWidth="1"/>
+    <col min="15" max="15" width="13.125" style="6" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-    </row>
-    <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+    </row>
+    <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="M3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="39" t="s">
+      <c r="O3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="18" t="s">
         <v>13</v>
       </c>
@@ -1046,14 +1035,14 @@
       <c r="J4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="38"/>
-    </row>
-    <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="36"/>
+    </row>
+    <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="7"/>
@@ -1071,11 +1060,11 @@
       <c r="O5" s="8"/>
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -1091,19 +1080,19 @@
       <c r="O6" s="14"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O7" s="16"/>
       <c r="P7" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="P8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" s="5" t="s">
         <v>16</v>
@@ -1140,41 +1129,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="32" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="59" style="32" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="32" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="32"/>
+    <col min="1" max="1" width="5.375" style="30" customWidth="1"/>
+    <col min="2" max="2" width="27.25" style="30" customWidth="1"/>
+    <col min="3" max="3" width="59" style="30" customWidth="1"/>
+    <col min="4" max="4" width="17.125" style="31" customWidth="1"/>
+    <col min="5" max="5" width="12.875" style="30" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:5" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-    </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:5" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
-      <c r="D2" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="31"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -1193,42 +1183,42 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="35" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
       <c r="D4" s="25"/>
       <c r="E4" s="20"/>
     </row>
-    <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+    <row r="5" spans="1:5" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-    </row>
-    <row r="6" spans="1:5" s="21" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="27"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" spans="1:5" s="21" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="26"/>
       <c r="E6" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="28"/>
+    <row r="7" spans="1:5" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="D7" s="27"/>
       <c r="E7" s="23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
+    <row r="8" spans="1:5" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="28"/>
+      <c r="C8" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="27"/>
       <c r="E8" s="19" t="s">
         <v>19</v>
       </c>
@@ -1236,10 +1226,10 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="92" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[dattt] update template thoi su
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateTS.xlsx
+++ b/ATV_Allowance/Templates/TemplateTS.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\job\ATV-Allowance\ATV-Allowance\ATV_Allowance\Templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="6960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PV" sheetId="1" r:id="rId1"/>
@@ -128,9 +123,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -299,7 +294,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -340,13 +335,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,7 +377,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -700,7 +695,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -713,31 +708,32 @@
   </sheetPr>
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="10" customWidth="1"/>
-    <col min="2" max="3" width="27.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" style="2" customWidth="1"/>
-    <col min="14" max="15" width="10.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="27" customWidth="1"/>
-    <col min="17" max="17" width="15" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="9.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="2" customWidth="1"/>
+    <col min="14" max="15" width="10.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="21.77734375" style="27" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -758,7 +754,7 @@
       <c r="P1" s="39"/>
       <c r="Q1" s="39"/>
     </row>
-    <row r="2" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>20</v>
       </c>
@@ -779,7 +775,7 @@
       <c r="P2" s="42"/>
       <c r="Q2" s="42"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
@@ -818,7 +814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
@@ -853,7 +849,7 @@
       <c r="P4" s="41"/>
       <c r="Q4" s="40"/>
     </row>
-    <row r="5" spans="1:17" s="6" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="6" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -872,7 +868,7 @@
       <c r="P5" s="25"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="38" t="s">
         <v>7</v>
       </c>
@@ -893,19 +889,19 @@
       <c r="P6" s="8"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P7" s="26"/>
       <c r="Q7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="Q8" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="16" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="16" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B9" s="37" t="s">
         <v>16</v>
       </c>
@@ -950,31 +946,32 @@
   </sheetPr>
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="10" customWidth="1"/>
-    <col min="2" max="3" width="27.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.77734375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="31" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" style="2" customWidth="1"/>
-    <col min="14" max="15" width="10.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="27" customWidth="1"/>
-    <col min="17" max="17" width="15" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="9.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="2" customWidth="1"/>
+    <col min="14" max="15" width="10.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" style="27" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -995,7 +992,7 @@
       <c r="P1" s="39"/>
       <c r="Q1" s="39"/>
     </row>
-    <row r="2" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>20</v>
       </c>
@@ -1016,7 +1013,7 @@
       <c r="P2" s="42"/>
       <c r="Q2" s="42"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
@@ -1055,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
@@ -1090,7 +1087,7 @@
       <c r="P4" s="41"/>
       <c r="Q4" s="40"/>
     </row>
-    <row r="5" spans="1:17" s="6" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="6" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1109,7 +1106,7 @@
       <c r="P5" s="25"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="38" t="s">
         <v>7</v>
       </c>
@@ -1130,19 +1127,19 @@
       <c r="P6" s="8"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P7" s="26"/>
       <c r="Q7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="Q8" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="16" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="16" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B9" s="37" t="s">
         <v>16</v>
       </c>
@@ -1188,20 +1185,20 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" style="20" customWidth="1"/>
     <col min="3" max="3" width="59" style="20" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="20" customWidth="1"/>
     <col min="6" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -1210,7 +1207,7 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" spans="1:5" s="35" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="35" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>24</v>
       </c>
@@ -1219,7 +1216,7 @@
       <c r="D2" s="45"/>
       <c r="E2" s="45"/>
     </row>
-    <row r="3" spans="1:5" s="23" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="23" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="31" t="s">
         <v>23</v>
       </c>
@@ -1236,14 +1233,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32"/>
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
       <c r="D4" s="22"/>
       <c r="E4" s="32"/>
     </row>
-    <row r="5" spans="1:5" s="30" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="30" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
         <v>29</v>
       </c>
@@ -1252,19 +1249,19 @@
       <c r="D5" s="28"/>
       <c r="E5" s="29"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="19"/>
       <c r="E6" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="33" customFormat="1" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="33" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="D7" s="34"/>
       <c r="E7" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="24" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
DATTT - Add cong tac phi to Thoi Su
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateTS.xlsx
+++ b/ATV_Allowance/Templates/TemplateTS.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\job\ATV-Allowance\ATV-Allowance\ATV_Allowance\Templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="6960" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="PV" sheetId="1" r:id="rId1"/>
     <sheet name="CTV" sheetId="2" r:id="rId2"/>
     <sheet name="KHK" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>Đài Phát thanh - Truyền hình An Giang</t>
   </si>
@@ -123,12 +118,18 @@
   </si>
   <si>
     <t>Đơn vị</t>
+  </si>
+  <si>
+    <t>CTP</t>
+  </si>
+  <si>
+    <t>Điểm CTP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -278,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -378,6 +379,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -706,7 +713,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -717,10 +724,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -735,100 +742,108 @@
     <col min="8" max="8" width="7.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" style="2" customWidth="1"/>
-    <col min="14" max="15" width="10.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" style="27" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="2"/>
+    <col min="11" max="11" width="10" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" style="2" customWidth="1"/>
+    <col min="16" max="17" width="10.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" style="27" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:19" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-    </row>
-    <row r="2" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="44" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+    </row>
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42" t="s">
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="O3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="P3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="Q3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="R3" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="S3" s="44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
+    <row r="4" spans="1:19" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="38" t="s">
         <v>13</v>
       </c>
@@ -850,17 +865,23 @@
       <c r="J4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="42"/>
-    </row>
-    <row r="5" spans="1:17" s="6" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="44"/>
+    </row>
+    <row r="5" spans="1:19" s="6" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -876,15 +897,17 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="25"/>
+      <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="R5" s="25"/>
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -897,22 +920,24 @@
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
-    </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P7" s="26"/>
-      <c r="Q7" s="14" t="s">
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="1:19" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="26"/>
+      <c r="S7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="Q8" s="15" t="s">
+      <c r="S8" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="16" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="16" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="39" t="s">
         <v>16</v>
       </c>
@@ -922,27 +947,27 @@
       <c r="F9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="M9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="R9" s="18" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A1:S1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="D3:M3"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="A2:S2"/>
     <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -955,10 +980,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -973,100 +998,108 @@
     <col min="8" max="8" width="7.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" style="2" customWidth="1"/>
-    <col min="14" max="15" width="10.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" style="27" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="2"/>
+    <col min="11" max="11" width="11" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" style="2" customWidth="1"/>
+    <col min="16" max="17" width="10.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" style="27" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:19" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-    </row>
-    <row r="2" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="44" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+    </row>
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-    </row>
-    <row r="3" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+    </row>
+    <row r="3" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42" t="s">
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="O3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="P3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="Q3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="R3" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="S3" s="44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
+    <row r="4" spans="1:19" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="13" t="s">
         <v>13</v>
       </c>
@@ -1088,17 +1121,23 @@
       <c r="J4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="42"/>
-    </row>
-    <row r="5" spans="1:17" s="6" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="44"/>
+    </row>
+    <row r="5" spans="1:19" s="6" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1114,15 +1153,17 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="25"/>
+      <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="R5" s="25"/>
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -1135,22 +1176,24 @@
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
-    </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P7" s="26"/>
-      <c r="Q7" s="14" t="s">
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="1:19" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="26"/>
+      <c r="S7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="Q8" s="15" t="s">
+      <c r="S8" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="16" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="16" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="37" t="s">
         <v>16</v>
       </c>
@@ -1160,27 +1203,27 @@
       <c r="F9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="M9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="R9" s="18" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S3:S4"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="D3:M3"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
     <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1195,7 +1238,7 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1210,22 +1253,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" s="35" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:5" s="23" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
@@ -1252,11 +1295,11 @@
       <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" s="30" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="28"/>
       <c r="E5" s="29"/>
     </row>
@@ -1279,10 +1322,10 @@
       <c r="C8" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="48"/>
+      <c r="E8" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>